<commit_message>
Lista sección 14-1 Confiabilidad de Hardware :)
</commit_message>
<xml_diff>
--- a/Documentación/Tablas/11-1-4 Plan de pruebas de cada módulo (Hardware).xlsx
+++ b/Documentación/Tablas/11-1-4 Plan de pruebas de cada módulo (Hardware).xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274B9B3-9F19-459F-AF18-7B0E0ED2A5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2844DDAB-1D47-4A55-9906-7EFCD0617DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Logger" sheetId="2" r:id="rId1"/>
+    <sheet name="Base" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,63 +32,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
-  <si>
-    <t>Banco</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>BP-01</t>
-  </si>
-  <si>
-    <t>BP-02</t>
-  </si>
-  <si>
-    <t>BP-03</t>
-  </si>
-  <si>
-    <t>BP-04</t>
-  </si>
-  <si>
-    <t>BP-05</t>
-  </si>
-  <si>
-    <t>FOTO</t>
-  </si>
-  <si>
-    <t>\tabitem Penguin Logger.
-\tabitem Penguin Base.
-\tabitem Data Logger de alimentacíon.
-\tabitem Fuente regulada de 3.3V, capaz de entregar al menos 100mA.
-\tabitem Sensor de temperatura calibrado.
-\tabitem Cronómetro calibrado.
-\tabitem Recipiente con agua salada.</t>
-  </si>
-  <si>
-    <t>\tabitem Penguin Logger.
-\tabitem Batería utilizada.
-\tabitem Data Logger.</t>
-  </si>
-  <si>
-    <t>\tabitem Penguin Logger, sellado en su poteo.
-\tabitem Penguin Base.
-\tabitem Instrumentos de medición dimensional con resolución de al menos 1mm.
-\tabitem Balanza digital con resolución de al menos 0.1g.</t>
-  </si>
-  <si>
-    <t>\tabitem Penguin Logger, sellado en su poteo.
-\tabitem Penguin Base.
-\tabitem Cámara de presión calibrada, capaz de generar al menos 10bar de presión.
-\tabitem Manómetro calibrado.
-\tabitem Sensor de temperatura calibrado.
-\tabitem Recipiente con agua salada.</t>
-  </si>
-  <si>
-    <t>\tabitem Penguin Logger, sellado en su poteo y con datos.
-\tabitem Penguin Base.
-\tabitem Computadora con programa de recoleccíon de datos (PenGUI).</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>Microprocesador</t>
+  </si>
+  <si>
+    <t>Pilas</t>
+  </si>
+  <si>
+    <t>Interfaz de alimentación externa</t>
+  </si>
+  <si>
+    <t>Interfaz de comunicación serie</t>
+  </si>
+  <si>
+    <t>Sensor de conductividad</t>
+  </si>
+  <si>
+    <t>LED indicador</t>
+  </si>
+  <si>
+    <t>Plan de prueba</t>
+  </si>
+  <si>
+    <t>\tabitem Conectar las dos pilas a su conector dedicado en el dispositivo.
+\tabitem Verificar con un multímetro que la tensión medida entre ambas pilas es de $3,1V$.
+\tabitem Verificar con un multímetro que la tensión medida entre el negativo del conjunto de pilas y el cátodo del diodo $D_1$ está entre $2,6V$ y $2,8V$.</t>
+  </si>
+  <si>
+    <t>\tabitem Aplicar una tensión de $5V$ entre los conectores de alimentación externa.
+\tabitem Verificar con un multímetro que la tensión entre el pin externo negativo y la alimentación del microcontrolador $V_{cc}$ está entre $3V$ y $3,3V$.
+\tabitem Verificar con un multímetro que la tensión entre el pin externo negativo y el pin P4.2 del microcontrolador (Base Detect) está entre $3V$ y $3,3V$.</t>
+  </si>
+  <si>
+    <t>\tabitem Cortocircuitar los conectores externos del dispositivo en modo de medición.
+\tabitem Verificar con un multímetro que la tensión en el pin P1.5 esté entre $2,25V$ y la tensión de alimentación $V_{cc}$.</t>
+  </si>
+  <si>
+    <t>\tabitem Aplicar una tensión de $3V$ a $R_4$.
+\tabitem Verificar que el LED se enciende y que su brillo es adecuado.
+\tabitem Verificar con un multímetro que la corriente que circula por el LED no supere los $5mA$.</t>
+  </si>
+  <si>
+    <t>Circuito de generación de flancos</t>
+  </si>
+  <si>
+    <t>\tabitem Programar el microcontrolador usando el conector de programación dedicado.
+\tabitem Utilizar un programa que configure los pines de salida y de comunicación.
+\tabitem Verificar que el programa cargue correctamente.
+\tabitem Aplicar una señal digital alta a los pines de entrada.
+\tabitem Verificar con un multímetro que los pines de salida reflejan una señal digital alta.
+\tabitem Utilizar un osciloscopio con analizador de tramas para verificar que el mensaje enviado y recibido sea el correcto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\tabitem Aplicar una tensión de $3,3V$ a $R_{g_1}$ y a $R_{g_2}$.
+\tabitem Verificar con un multímetro que la tensión en $V_{ext}$ es de $5V$.
+\tabitem Verificar con un multímetro que la tensión en $RX$ (logger) sigue siempre a $TX$ (base). </t>
+  </si>
+  <si>
+    <t>\tabitem Aplicar una tensión de $3,3V$ a $R_1$, $R_2$ y $R_3$, .
+\tabitem Verificar que el LED RGB se enciende y que su brillo es adecuado.
+\tabitem Verificar con un multímetro que la corriente que circula por el LED no supere los $5mA$.</t>
+  </si>
+  <si>
+    <t>\tabitem Utilizar una placa de evaluación MSP430FR2433 LaunchPad para programar el microcontrolador usando el conector de programación dedicado.
+\tabitem Utilizar un programa que configure las entradas y salidas.
+\tabitem Verificar que el programa cargue correctamente.
+\tabitem Aplicar una señal digital alta a los pines de entrada.
+\tabitem Utilizar un multímetro para verificar que los pines de salida reflejan una señal digital alta.</t>
+  </si>
+  <si>
+    <t>\tabitem Cargar un programa que configure los pines P1.4 y P1.5 como transmisión y recepción de una interfaz de comunicación UART.
+\tabitem Utilizar un osciloscopio con analizador de tramas para verificar que el mensaje enviado y recibido sea el correcto.</t>
   </si>
 </sst>
 </file>
@@ -138,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,95 +180,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -537,86 +482,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAD9908-3DB8-46A4-94BE-5CD81246CF66}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="73.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18E9219-6DCB-480B-A73A-439442A5E26A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>